<commit_message>
Filled out the front-matter more.
</commit_message>
<xml_diff>
--- a/AlternativeApproach.xlsx
+++ b/AlternativeApproach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\GitHub\MoreTraceability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876B3AF6-1DB5-4214-9FAE-669DB5187054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B044CFB5-0009-4B4A-9211-7A78DCB4DA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="798" xr2:uid="{B9646992-58BC-44A8-9040-42DC40CCACD9}"/>
   </bookViews>
@@ -16,24 +16,24 @@
     <sheet name="FrontMatter" sheetId="15" r:id="rId1"/>
     <sheet name="URS←Plan→Report" sheetId="3" r:id="rId2"/>
     <sheet name="Bench_Validation_Mapping" sheetId="9" r:id="rId3"/>
-    <sheet name="Report" sheetId="1" r:id="rId4"/>
+    <sheet name="Metadata" sheetId="1" r:id="rId4"/>
     <sheet name="URS_Total" sheetId="13" state="hidden" r:id="rId5"/>
     <sheet name="RemoveFromURS" sheetId="14" r:id="rId6"/>
     <sheet name="URS_Uncovered" sheetId="6" r:id="rId7"/>
     <sheet name="URS_Bench_Validate" sheetId="7" state="hidden" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FrontMatter!$A$5:$F$49</definedName>
-    <definedName name="_fName">Report!$B$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FrontMatter!$A$8:$F$51</definedName>
+    <definedName name="_fName">Metadata!$B$7</definedName>
     <definedName name="_nBRC">URS_Bench_Validate!$B$1</definedName>
     <definedName name="_tBenchVal">OFFSET(URS_Bench_Validate!$A$4,0,0,_nBRC,3)</definedName>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">Bench_Validation_Mapping!$A$1:$E$3172</definedName>
     <definedName name="ExternalData_2" localSheetId="1" hidden="1">URS←Plan→Report!$A$1:$F$98</definedName>
     <definedName name="ExternalData_5" localSheetId="6" hidden="1">URS_Uncovered!$A$1:$B$216</definedName>
     <definedName name="ExternalData_8" localSheetId="4" hidden="1">URS_Total!$A$1:$B$291</definedName>
-    <definedName name="FromArray_1">_xlfn.ANCHORARRAY(Report!$B$7)</definedName>
+    <definedName name="FromArray_1">_xlfn.ANCHORARRAY(Metadata!$B$7)</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Bench_Validation_Mapping[]</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">FrontMatter!$A$1:$M$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">FrontMatter!$A$1:$I$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">URS_Plan_Report[#All]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Bench_Validation_Mapping!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">URS←Plan→Report!$1:$1</definedName>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17707" uniqueCount="1824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17727" uniqueCount="1842">
   <si>
     <t>FROM:</t>
   </si>
@@ -5618,6 +5618,60 @@
   </si>
   <si>
     <t>Utica CIC Validation Matrices</t>
+  </si>
+  <si>
+    <t>Bench Validation</t>
+  </si>
+  <si>
+    <t>SyRS</t>
+  </si>
+  <si>
+    <t>CIC</t>
+  </si>
+  <si>
+    <t>GHz</t>
+  </si>
+  <si>
+    <t>GigaHertz</t>
+  </si>
+  <si>
+    <t>Completely in Canal</t>
+  </si>
+  <si>
+    <t>System Requirement Specification</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>User Need</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>A hearing aid wearer or a hearing aid professoinal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An characteristic of the hearing aid that is required by the user </t>
+  </si>
+  <si>
+    <t>to make use of the hearing aid.</t>
+  </si>
+  <si>
+    <t>Applying system tests to validate some user needs.</t>
   </si>
 </sst>
 </file>
@@ -5979,7 +6033,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6009,6 +6063,21 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="9" applyFill="1"/>
     <xf numFmtId="15" fontId="1" fillId="9" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="20% - Accent1 2" xfId="20" xr:uid="{C2DEE543-1A64-4ED9-AFEE-49DCCF23A27D}"/>
@@ -6047,6 +6116,72 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -6124,72 +6259,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -6276,16 +6345,16 @@
       <tableStyleElement type="firstColumnStripe" dxfId="28"/>
     </tableStyle>
     <tableStyle name="Biegert Standard 2" table="0" count="4" xr9:uid="{832498C2-108D-49C5-8C4C-08D4A9D6AECD}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstColumn" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="27"/>
+      <tableStyleElement type="totalRow" dxfId="26"/>
+      <tableStyleElement type="firstColumn" dxfId="25"/>
+      <tableStyleElement type="firstRowStripe" dxfId="24"/>
     </tableStyle>
     <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{5137A684-FC5E-482B-B17B-7D54AF6E2ECA}">
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="totalRow" dxfId="22"/>
+      <tableStyleElement type="firstColumn" dxfId="21"/>
+      <tableStyleElement type="firstRowStripe" dxfId="20"/>
     </tableStyle>
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{6599F34C-6A9E-4238-B66C-9E696F7A2B73}"/>
   </tableStyles>
@@ -6304,62 +6373,506 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Group 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B5EB987-B3B1-AA7A-D516-FF9DF2CD3B49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1438275" y="4953000"/>
+          <a:ext cx="4219575" cy="1114425"/>
+          <a:chOff x="2028825" y="4229100"/>
+          <a:chExt cx="5715000" cy="1619250"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EB985FC-CD1B-D2CB-455D-367B9DBBC3F0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2028825" y="4229100"/>
+            <a:ext cx="1428750" cy="647700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Utica User Requirement Specificaton               </a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9E0AF03-0372-411E-B132-497F2240149B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4171950" y="4229100"/>
+            <a:ext cx="1428750" cy="647700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Utica</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> 2.4 GHz Test Plan</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>              </a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Rectangle 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31AA4DC5-8431-4DCF-AF75-59BEE96A0D8D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6315075" y="4229100"/>
+            <a:ext cx="1428750" cy="647700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Utica</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> 2.4 GHz Test Report</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>              </a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF713AF5-485C-4A68-1B8D-BA32B5621940}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="3"/>
+            <a:endCxn id="4" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3457575" y="4552950"/>
+            <a:ext cx="714375" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7F8B774-D414-62BD-C620-40DD56895ECE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="4" idx="3"/>
+            <a:endCxn id="5" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5600700" y="4552950"/>
+            <a:ext cx="714375" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B4DC3B5-E77C-4726-826B-F324AF6DCDF4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4171950" y="5200650"/>
+            <a:ext cx="1428750" cy="647700"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Utica</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> SyRS Trace Matrix</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="12" name="Connector: Elbow 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8452B54E-7107-DF7C-8F19-B0B879BEFC74}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="3" idx="3"/>
+            <a:endCxn id="10" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3457575" y="4552950"/>
+            <a:ext cx="714375" cy="971550"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="14" name="Connector: Elbow 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B917A2C-041D-0812-C1D7-109606CD46A3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="10" idx="3"/>
+            <a:endCxn id="5" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="5600700" y="4876800"/>
+            <a:ext cx="1428750" cy="647700"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2">
+        <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EB985FC-CD1B-D2CB-455D-367B9DBBC3F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA80BA51-D24C-C14E-7C74-E37E5DDDD5A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
+        <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1514475" y="3562350"/>
-          <a:ext cx="1428750" cy="647700"/>
+          <a:off x="838200" y="428625"/>
+          <a:ext cx="6143626" cy="600076"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Utica User Requirement Specificaton               </a:t>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>This document presents the validation traceability matrices for the Utica</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> 2.4 GHz CIC development.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t> This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> report was generated in Excel using requirement exports from Polarion.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6367,436 +6880,300 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 3">
+        <xdr:cNvPr id="8" name="TextBox 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9E0AF03-0372-411E-B132-497F2240149B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C9B2538-61E4-8872-0F9A-1AE8D075C083}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvSpPr/>
+        <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3657600" y="3562350"/>
-          <a:ext cx="1428750" cy="647700"/>
+          <a:off x="876301" y="3152774"/>
+          <a:ext cx="6095999" cy="1790701"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="dk1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Utica</a:t>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Four documents were</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> 2.4 GHz Test Plan</a:t>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> used to generate the validation matrices:</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1000" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:tabLst>
+              <a:tab pos="365760" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>              </a:t>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>●	User Requirement Specification</a:t>
           </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>	Contains user needs.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:tabLst>
+              <a:tab pos="365760" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>●	Test Plan</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	Validation test plan for user needs.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst>
+              <a:tab pos="365760" algn="l"/>
+            </a:tabLst>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>●	Test Report</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	Contains results from performing the tests called out by the test plan.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst>
+              <a:tab pos="365760" algn="l"/>
+            </a:tabLst>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>●	SyRS Trace Matrix</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	Some user requirements were tested separately from Clinical Research.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:effectLst/>
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst>
+              <a:tab pos="365760" algn="l"/>
+            </a:tabLst>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:tabLst>
+              <a:tab pos="365760" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1000" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31AA4DC5-8431-4DCF-AF75-59BEE96A0D8D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5800725" y="3562350"/>
-          <a:ext cx="1428750" cy="647700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Utica</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> 2.4 GHz Test Report</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>              </a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF713AF5-485C-4A68-1B8D-BA32B5621940}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="3"/>
-          <a:endCxn id="4" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2943225" y="3886200"/>
-          <a:ext cx="714375" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7F8B774-D414-62BD-C620-40DD56895ECE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="4" idx="3"/>
-          <a:endCxn id="5" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5086350" y="3886200"/>
-          <a:ext cx="714375" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B4DC3B5-E77C-4726-826B-F324AF6DCDF4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3657600" y="4533900"/>
-          <a:ext cx="1428750" cy="647700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Utica</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> SyRS Trace Matrix</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Connector: Elbow 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8452B54E-7107-DF7C-8F19-B0B879BEFC74}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="3"/>
-          <a:endCxn id="10" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2943225" y="3886200"/>
-          <a:ext cx="714375" cy="971550"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Connector: Elbow 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B917A2C-041D-0812-C1D7-109606CD46A3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="10" idx="3"/>
-          <a:endCxn id="5" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5086350" y="4210050"/>
-          <a:ext cx="1428750" cy="647700"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6855,15 +7232,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8B90B28E-9024-408E-B7DD-9DB2973675B9}" name="URS_Plan_Report" displayName="URS_Plan_Report" ref="A1:F98" tableType="queryTable" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8B90B28E-9024-408E-B7DD-9DB2973675B9}" name="URS_Plan_Report" displayName="URS_Plan_Report" ref="A1:F98" tableType="queryTable" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:F98" xr:uid="{8B90B28E-9024-408E-B7DD-9DB2973675B9}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E910450F-A0B8-422A-ADA7-86102213337D}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{06AE4070-13DF-4862-B3A7-D1B13319C4B0}" uniqueName="2" name="URS_Title" queryTableFieldId="2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{BA7B501B-FDC1-4FC4-B898-12C84701A8E4}" uniqueName="3" name="Test_Plan_ID" queryTableFieldId="3" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{06A6D0F1-68DE-42F5-864F-A06E59885CF8}" uniqueName="4" name="Test_Plan_Title" queryTableFieldId="4" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{90E9C3DB-C986-42B6-B868-3B5E8BA95577}" uniqueName="5" name="Report_ID" queryTableFieldId="5" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{B691F662-0FCA-4580-8F97-1129A9488E46}" uniqueName="6" name="Report_ID_Title" queryTableFieldId="6" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{E910450F-A0B8-422A-ADA7-86102213337D}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{06AE4070-13DF-4862-B3A7-D1B13319C4B0}" uniqueName="2" name="URS_Title" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{BA7B501B-FDC1-4FC4-B898-12C84701A8E4}" uniqueName="3" name="Test_Plan_ID" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{06A6D0F1-68DE-42F5-864F-A06E59885CF8}" uniqueName="4" name="Test_Plan_Title" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{90E9C3DB-C986-42B6-B868-3B5E8BA95577}" uniqueName="5" name="Report_ID" queryTableFieldId="5" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{B691F662-0FCA-4580-8F97-1129A9488E46}" uniqueName="6" name="Report_ID_Title" queryTableFieldId="6" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6873,11 +7250,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{21447C5E-D138-48B8-81A1-CFD1001CCF28}" name="Bench_Validation_Mapping" displayName="Bench_Validation_Mapping" ref="A1:E3172" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E3172" xr:uid="{21447C5E-D138-48B8-81A1-CFD1001CCF28}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8371926A-097A-427B-BE67-2F30749B541C}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{1E7800CE-0B06-469A-A591-97D10BE290BF}" uniqueName="2" name="Title" queryTableFieldId="2" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{5FB67C02-E8A5-43ED-B0FF-97CEA52E91D5}" uniqueName="3" name="Test Case" queryTableFieldId="3" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{2A2F4866-25AA-4E13-8EC2-D1C21A743A89}" uniqueName="4" name="Test Report" queryTableFieldId="4" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{1B676804-D802-4732-A90B-AC7D3C1A499D}" uniqueName="5" name="Test Result" queryTableFieldId="5" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{8371926A-097A-427B-BE67-2F30749B541C}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{1E7800CE-0B06-469A-A591-97D10BE290BF}" uniqueName="2" name="Title" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{5FB67C02-E8A5-43ED-B0FF-97CEA52E91D5}" uniqueName="3" name="Test Case" queryTableFieldId="3" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{2A2F4866-25AA-4E13-8EC2-D1C21A743A89}" uniqueName="4" name="Test Report" queryTableFieldId="4" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{1B676804-D802-4732-A90B-AC7D3C1A499D}" uniqueName="5" name="Test Result" queryTableFieldId="5" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6887,8 +7264,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D7396E22-7624-45A3-AAB9-73422A0FA226}" name="URS_Total" displayName="URS_Total" ref="A1:B291" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B291" xr:uid="{D7396E22-7624-45A3-AAB9-73422A0FA226}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{277B1261-3060-4A34-8604-0129EAB39E9A}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{AA05DE6F-E53C-4C50-A77F-48B0626D6BD4}" uniqueName="4" name="Title" queryTableFieldId="4" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{277B1261-3060-4A34-8604-0129EAB39E9A}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{AA05DE6F-E53C-4C50-A77F-48B0626D6BD4}" uniqueName="4" name="Title" queryTableFieldId="4" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6898,9 +7275,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C98B7286-DFC4-48D9-A7D5-D332086D9421}" name="URS_Uncovered" displayName="URS_Uncovered" ref="A1:C216" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:C216" xr:uid="{C98B7286-DFC4-48D9-A7D5-D332086D9421}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{29BE8571-0E0E-4F25-A5C5-DBE272610AA6}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{E66AF785-C1A6-4595-89FD-F11C00D8041A}" uniqueName="2" name="Title" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{AA585E2E-875E-4BF5-883B-78E2AC510C64}" uniqueName="3" name="Bucket" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{29BE8571-0E0E-4F25-A5C5-DBE272610AA6}" uniqueName="1" name="URS_ID" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{E66AF785-C1A6-4595-89FD-F11C00D8041A}" uniqueName="2" name="Title" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{AA585E2E-875E-4BF5-883B-78E2AC510C64}" uniqueName="3" name="Bucket" queryTableFieldId="3" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7153,18 +7530,19 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1822</v>
       </c>
@@ -7172,7 +7550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -7180,25 +7558,132 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="3" spans="1:8" ht="2.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>1819</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="1:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="32" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="32" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="32" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="33" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="31"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>1820</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="16" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+    </row>
+    <row r="17" spans="1:3" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="14" t="s">
+        <v>1824</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="14" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="14"/>
+      <c r="C20" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>1821</v>
       </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LUtica CIC Validation Report</oddHeader>
     <oddFooter>&amp;LFront Matter&amp;CStarkey Confidential
@@ -7216,10 +7701,10 @@
   </sheetPr>
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection activeCell="K17" sqref="K17"/>
-      <selection pane="topRight" activeCell="K17" sqref="K17"/>
+      <selection activeCell="G49" sqref="G49"/>
+      <selection pane="topRight" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9184,11 +9669,12 @@
       </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LUtica CIC Validation Report</oddHeader>
-    <oddFooter>&amp;LTrace: URS → Plan → Report&amp;CStarkey Confidential
+    <oddFooter>&amp;LFront Matter&amp;CStarkey Confidential
 &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
@@ -9205,8 +9691,8 @@
   </sheetPr>
   <dimension ref="A1:E3172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -63143,11 +63629,12 @@
       </c>
     </row>
   </sheetData>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LUtica CIC Validation Report</oddHeader>
-    <oddFooter>&amp;LUTICA CIC Bench Validation&amp;CStarkey Confidential
+    <oddFooter>&amp;LFront Matter&amp;CStarkey Confidential
 &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
@@ -63165,7 +63652,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>

</xml_diff>